<commit_message>
V1.2 (storage fix + skipper fix)
</commit_message>
<xml_diff>
--- a/NameFile.xlsx
+++ b/NameFile.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S62"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2112,1649 +2112,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>44835</v>
-      </c>
-      <c r="B32" t="n">
-        <v>22</v>
-      </c>
-      <c r="C32" t="n">
-        <v>1825</v>
-      </c>
-      <c r="D32" t="n">
-        <v>0</v>
-      </c>
-      <c r="E32" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" t="n">
-        <v>1</v>
-      </c>
-      <c r="G32" t="n">
-        <v>1838</v>
-      </c>
-      <c r="H32" t="n">
-        <v>11</v>
-      </c>
-      <c r="I32" t="n">
-        <v>1357.68</v>
-      </c>
-      <c r="J32" t="n">
-        <v>0</v>
-      </c>
-      <c r="K32" t="n">
-        <v>0</v>
-      </c>
-      <c r="L32" t="n">
-        <v>0</v>
-      </c>
-      <c r="M32" t="n">
-        <v>0</v>
-      </c>
-      <c r="N32" t="n">
-        <v>37</v>
-      </c>
-      <c r="O32" t="n">
-        <v>2213.04</v>
-      </c>
-      <c r="P32" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q32" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>44836</v>
-      </c>
-      <c r="B33" t="n">
-        <v>8</v>
-      </c>
-      <c r="C33" t="n">
-        <v>1920.35</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0</v>
-      </c>
-      <c r="E33" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" t="n">
-        <v>1</v>
-      </c>
-      <c r="G33" t="n">
-        <v>1866</v>
-      </c>
-      <c r="H33" t="n">
-        <v>10</v>
-      </c>
-      <c r="I33" t="n">
-        <v>1343.48</v>
-      </c>
-      <c r="J33" t="n">
-        <v>0</v>
-      </c>
-      <c r="K33" t="n">
-        <v>0</v>
-      </c>
-      <c r="L33" t="n">
-        <v>0</v>
-      </c>
-      <c r="M33" t="n">
-        <v>0</v>
-      </c>
-      <c r="N33" t="n">
-        <v>57</v>
-      </c>
-      <c r="O33" t="n">
-        <v>1583.56</v>
-      </c>
-      <c r="P33" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q33" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>44837</v>
-      </c>
-      <c r="B34" t="n">
-        <v>8</v>
-      </c>
-      <c r="C34" t="n">
-        <v>1920.35</v>
-      </c>
-      <c r="D34" t="n">
-        <v>0</v>
-      </c>
-      <c r="E34" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" t="n">
-        <v>1</v>
-      </c>
-      <c r="G34" t="n">
-        <v>1938</v>
-      </c>
-      <c r="H34" t="n">
-        <v>10</v>
-      </c>
-      <c r="I34" t="n">
-        <v>1343.48</v>
-      </c>
-      <c r="J34" t="n">
-        <v>0</v>
-      </c>
-      <c r="K34" t="n">
-        <v>0</v>
-      </c>
-      <c r="L34" t="n">
-        <v>0</v>
-      </c>
-      <c r="M34" t="n">
-        <v>0</v>
-      </c>
-      <c r="N34" t="n">
-        <v>57</v>
-      </c>
-      <c r="O34" t="n">
-        <v>1583.56</v>
-      </c>
-      <c r="P34" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q34" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>44838</v>
-      </c>
-      <c r="B35" t="n">
-        <v>19</v>
-      </c>
-      <c r="C35" t="n">
-        <v>1920.35</v>
-      </c>
-      <c r="D35" t="n">
-        <v>0</v>
-      </c>
-      <c r="E35" t="n">
-        <v>0</v>
-      </c>
-      <c r="F35" t="n">
-        <v>2</v>
-      </c>
-      <c r="G35" t="n">
-        <v>1938</v>
-      </c>
-      <c r="H35" t="n">
-        <v>0</v>
-      </c>
-      <c r="I35" t="n">
-        <v>0</v>
-      </c>
-      <c r="J35" t="n">
-        <v>5</v>
-      </c>
-      <c r="K35" t="n">
-        <v>1274</v>
-      </c>
-      <c r="L35" t="n">
-        <v>0</v>
-      </c>
-      <c r="M35" t="n">
-        <v>0</v>
-      </c>
-      <c r="N35" t="n">
-        <v>20</v>
-      </c>
-      <c r="O35" t="n">
-        <v>419.03</v>
-      </c>
-      <c r="P35" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q35" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>44839</v>
-      </c>
-      <c r="B36" t="n">
-        <v>22</v>
-      </c>
-      <c r="C36" t="n">
-        <v>1825</v>
-      </c>
-      <c r="D36" t="n">
-        <v>0</v>
-      </c>
-      <c r="E36" t="n">
-        <v>0</v>
-      </c>
-      <c r="F36" t="n">
-        <v>2</v>
-      </c>
-      <c r="G36" t="n">
-        <v>1477</v>
-      </c>
-      <c r="H36" t="n">
-        <v>0</v>
-      </c>
-      <c r="I36" t="n">
-        <v>0</v>
-      </c>
-      <c r="J36" t="n">
-        <v>12</v>
-      </c>
-      <c r="K36" t="n">
-        <v>1818</v>
-      </c>
-      <c r="L36" t="n">
-        <v>0</v>
-      </c>
-      <c r="M36" t="n">
-        <v>0</v>
-      </c>
-      <c r="N36" t="n">
-        <v>20</v>
-      </c>
-      <c r="O36" t="n">
-        <v>419.03</v>
-      </c>
-      <c r="P36" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q36" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>44840</v>
-      </c>
-      <c r="B37" t="n">
-        <v>19</v>
-      </c>
-      <c r="C37" t="n">
-        <v>1825</v>
-      </c>
-      <c r="D37" t="n">
-        <v>0</v>
-      </c>
-      <c r="E37" t="n">
-        <v>0</v>
-      </c>
-      <c r="F37" t="n">
-        <v>2</v>
-      </c>
-      <c r="G37" t="n">
-        <v>1477.3</v>
-      </c>
-      <c r="H37" t="n">
-        <v>0</v>
-      </c>
-      <c r="I37" t="n">
-        <v>0</v>
-      </c>
-      <c r="J37" t="n">
-        <v>11</v>
-      </c>
-      <c r="K37" t="n">
-        <v>1818</v>
-      </c>
-      <c r="L37" t="n">
-        <v>0</v>
-      </c>
-      <c r="M37" t="n">
-        <v>0</v>
-      </c>
-      <c r="N37" t="n">
-        <v>20</v>
-      </c>
-      <c r="O37" t="n">
-        <v>419.03</v>
-      </c>
-      <c r="P37" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q37" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>44841</v>
-      </c>
-      <c r="B38" t="n">
-        <v>25</v>
-      </c>
-      <c r="C38" t="n">
-        <v>1914</v>
-      </c>
-      <c r="D38" t="n">
-        <v>0</v>
-      </c>
-      <c r="E38" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" t="n">
-        <v>2</v>
-      </c>
-      <c r="G38" t="n">
-        <v>1504.78</v>
-      </c>
-      <c r="H38" t="n">
-        <v>11</v>
-      </c>
-      <c r="I38" t="n">
-        <v>1343.48</v>
-      </c>
-      <c r="J38" t="n">
-        <v>12</v>
-      </c>
-      <c r="K38" t="n">
-        <v>1538.59</v>
-      </c>
-      <c r="L38" t="n">
-        <v>0</v>
-      </c>
-      <c r="M38" t="n">
-        <v>0</v>
-      </c>
-      <c r="N38" t="n">
-        <v>20</v>
-      </c>
-      <c r="O38" t="n">
-        <v>419.03</v>
-      </c>
-      <c r="P38" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q38" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>44842</v>
-      </c>
-      <c r="B39" t="n">
-        <v>32</v>
-      </c>
-      <c r="C39" t="n">
-        <v>1914</v>
-      </c>
-      <c r="D39" t="n">
-        <v>0</v>
-      </c>
-      <c r="E39" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" t="n">
-        <v>0</v>
-      </c>
-      <c r="G39" t="n">
-        <v>0</v>
-      </c>
-      <c r="H39" t="n">
-        <v>11</v>
-      </c>
-      <c r="I39" t="n">
-        <v>1343.48</v>
-      </c>
-      <c r="J39" t="n">
-        <v>15</v>
-      </c>
-      <c r="K39" t="n">
-        <v>1566.07</v>
-      </c>
-      <c r="L39" t="n">
-        <v>0</v>
-      </c>
-      <c r="M39" t="n">
-        <v>0</v>
-      </c>
-      <c r="N39" t="n">
-        <v>20</v>
-      </c>
-      <c r="O39" t="n">
-        <v>419.03</v>
-      </c>
-      <c r="P39" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q39" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="n">
-        <v>44843</v>
-      </c>
-      <c r="B40" t="n">
-        <v>24</v>
-      </c>
-      <c r="C40" t="n">
-        <v>1362.33</v>
-      </c>
-      <c r="D40" t="n">
-        <v>0</v>
-      </c>
-      <c r="E40" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" t="n">
-        <v>0</v>
-      </c>
-      <c r="G40" t="n">
-        <v>0</v>
-      </c>
-      <c r="H40" t="n">
-        <v>11</v>
-      </c>
-      <c r="I40" t="n">
-        <v>1343.48</v>
-      </c>
-      <c r="J40" t="n">
-        <v>18</v>
-      </c>
-      <c r="K40" t="n">
-        <v>1530</v>
-      </c>
-      <c r="L40" t="n">
-        <v>0</v>
-      </c>
-      <c r="M40" t="n">
-        <v>0</v>
-      </c>
-      <c r="N40" t="n">
-        <v>0</v>
-      </c>
-      <c r="O40" t="n">
-        <v>0</v>
-      </c>
-      <c r="P40" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q40" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="1" t="n">
-        <v>44844</v>
-      </c>
-      <c r="B41" t="n">
-        <v>16</v>
-      </c>
-      <c r="C41" t="n">
-        <v>1825</v>
-      </c>
-      <c r="D41" t="n">
-        <v>0</v>
-      </c>
-      <c r="E41" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" t="n">
-        <v>0</v>
-      </c>
-      <c r="G41" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" t="n">
-        <v>11</v>
-      </c>
-      <c r="I41" t="n">
-        <v>1343.48</v>
-      </c>
-      <c r="J41" t="n">
-        <v>16</v>
-      </c>
-      <c r="K41" t="n">
-        <v>1647.71</v>
-      </c>
-      <c r="L41" t="n">
-        <v>0</v>
-      </c>
-      <c r="M41" t="n">
-        <v>0</v>
-      </c>
-      <c r="N41" t="n">
-        <v>15</v>
-      </c>
-      <c r="O41" t="n">
-        <v>1824</v>
-      </c>
-      <c r="P41" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q41" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="n">
-        <v>44845</v>
-      </c>
-      <c r="B42" t="n">
-        <v>20</v>
-      </c>
-      <c r="C42" t="n">
-        <v>1825</v>
-      </c>
-      <c r="D42" t="n">
-        <v>0</v>
-      </c>
-      <c r="E42" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" t="n">
-        <v>1</v>
-      </c>
-      <c r="G42" t="n">
-        <v>1477.3</v>
-      </c>
-      <c r="H42" t="n">
-        <v>0</v>
-      </c>
-      <c r="I42" t="n">
-        <v>1826.09</v>
-      </c>
-      <c r="J42" t="n">
-        <v>16</v>
-      </c>
-      <c r="K42" t="n">
-        <v>1212</v>
-      </c>
-      <c r="L42" t="n">
-        <v>0</v>
-      </c>
-      <c r="M42" t="n">
-        <v>0</v>
-      </c>
-      <c r="N42" t="n">
-        <v>15</v>
-      </c>
-      <c r="O42" t="n">
-        <v>1824</v>
-      </c>
-      <c r="P42" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q42" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="1" t="n">
-        <v>44846</v>
-      </c>
-      <c r="B43" t="n">
-        <v>19</v>
-      </c>
-      <c r="C43" t="n">
-        <v>1823</v>
-      </c>
-      <c r="D43" t="n">
-        <v>0</v>
-      </c>
-      <c r="E43" t="n">
-        <v>0</v>
-      </c>
-      <c r="F43" t="n">
-        <v>1</v>
-      </c>
-      <c r="G43" t="n">
-        <v>1504.78</v>
-      </c>
-      <c r="H43" t="n">
-        <v>0</v>
-      </c>
-      <c r="I43" t="n">
-        <v>1826.09</v>
-      </c>
-      <c r="J43" t="n">
-        <v>16</v>
-      </c>
-      <c r="K43" t="n">
-        <v>1212.46</v>
-      </c>
-      <c r="L43" t="n">
-        <v>0</v>
-      </c>
-      <c r="M43" t="n">
-        <v>0</v>
-      </c>
-      <c r="N43" t="n">
-        <v>0</v>
-      </c>
-      <c r="O43" t="n">
-        <v>0</v>
-      </c>
-      <c r="P43" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q43" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="1" t="n">
-        <v>44847</v>
-      </c>
-      <c r="B44" t="n">
-        <v>16</v>
-      </c>
-      <c r="C44" t="n">
-        <v>1865</v>
-      </c>
-      <c r="D44" t="n">
-        <v>0</v>
-      </c>
-      <c r="E44" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" t="n">
-        <v>1</v>
-      </c>
-      <c r="G44" t="n">
-        <v>1477</v>
-      </c>
-      <c r="H44" t="n">
-        <v>0</v>
-      </c>
-      <c r="I44" t="n">
-        <v>0</v>
-      </c>
-      <c r="J44" t="n">
-        <v>16</v>
-      </c>
-      <c r="K44" t="n">
-        <v>1274</v>
-      </c>
-      <c r="L44" t="n">
-        <v>0</v>
-      </c>
-      <c r="M44" t="n">
-        <v>0</v>
-      </c>
-      <c r="N44" t="n">
-        <v>0</v>
-      </c>
-      <c r="O44" t="n">
-        <v>0</v>
-      </c>
-      <c r="P44" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q44" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="n">
-        <v>44848</v>
-      </c>
-      <c r="B45" t="n">
-        <v>31</v>
-      </c>
-      <c r="C45" t="n">
-        <v>1825</v>
-      </c>
-      <c r="D45" t="n">
-        <v>0</v>
-      </c>
-      <c r="E45" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" t="n">
-        <v>1</v>
-      </c>
-      <c r="G45" t="n">
-        <v>1477</v>
-      </c>
-      <c r="H45" t="n">
-        <v>11</v>
-      </c>
-      <c r="I45" t="n">
-        <v>1343.48</v>
-      </c>
-      <c r="J45" t="n">
-        <v>14</v>
-      </c>
-      <c r="K45" t="n">
-        <v>1625</v>
-      </c>
-      <c r="L45" t="n">
-        <v>0</v>
-      </c>
-      <c r="M45" t="n">
-        <v>0</v>
-      </c>
-      <c r="N45" t="n">
-        <v>0</v>
-      </c>
-      <c r="O45" t="n">
-        <v>0</v>
-      </c>
-      <c r="P45" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q45" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="n">
-        <v>44849</v>
-      </c>
-      <c r="B46" t="n">
-        <v>38</v>
-      </c>
-      <c r="C46" t="n">
-        <v>1725</v>
-      </c>
-      <c r="D46" t="n">
-        <v>0</v>
-      </c>
-      <c r="E46" t="n">
-        <v>0</v>
-      </c>
-      <c r="F46" t="n">
-        <v>1</v>
-      </c>
-      <c r="G46" t="n">
-        <v>1938.17</v>
-      </c>
-      <c r="H46" t="n">
-        <v>11</v>
-      </c>
-      <c r="I46" t="n">
-        <v>1343.48</v>
-      </c>
-      <c r="J46" t="n">
-        <v>17</v>
-      </c>
-      <c r="K46" t="n">
-        <v>1274</v>
-      </c>
-      <c r="L46" t="n">
-        <v>0</v>
-      </c>
-      <c r="M46" t="n">
-        <v>0</v>
-      </c>
-      <c r="N46" t="n">
-        <v>0</v>
-      </c>
-      <c r="O46" t="n">
-        <v>0</v>
-      </c>
-      <c r="P46" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q46" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="n">
-        <v>44850</v>
-      </c>
-      <c r="B47" t="n">
-        <v>19</v>
-      </c>
-      <c r="C47" t="n">
-        <v>1825</v>
-      </c>
-      <c r="D47" t="n">
-        <v>0</v>
-      </c>
-      <c r="E47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F47" t="n">
-        <v>1</v>
-      </c>
-      <c r="G47" t="n">
-        <v>1965.65</v>
-      </c>
-      <c r="H47" t="n">
-        <v>11</v>
-      </c>
-      <c r="I47" t="n">
-        <v>1343.48</v>
-      </c>
-      <c r="J47" t="n">
-        <v>12</v>
-      </c>
-      <c r="K47" t="n">
-        <v>1275</v>
-      </c>
-      <c r="L47" t="n">
-        <v>0</v>
-      </c>
-      <c r="M47" t="n">
-        <v>0</v>
-      </c>
-      <c r="N47" t="n">
-        <v>0</v>
-      </c>
-      <c r="O47" t="n">
-        <v>0</v>
-      </c>
-      <c r="P47" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q47" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="n">
-        <v>44851</v>
-      </c>
-      <c r="B48" t="n">
-        <v>25</v>
-      </c>
-      <c r="C48" t="n">
-        <v>1857</v>
-      </c>
-      <c r="D48" t="n">
-        <v>0</v>
-      </c>
-      <c r="E48" t="n">
-        <v>0</v>
-      </c>
-      <c r="F48" t="n">
-        <v>0</v>
-      </c>
-      <c r="G48" t="n">
-        <v>0</v>
-      </c>
-      <c r="H48" t="n">
-        <v>11</v>
-      </c>
-      <c r="I48" t="n">
-        <v>1343.48</v>
-      </c>
-      <c r="J48" t="n">
-        <v>17</v>
-      </c>
-      <c r="K48" t="n">
-        <v>1552</v>
-      </c>
-      <c r="L48" t="n">
-        <v>0</v>
-      </c>
-      <c r="M48" t="n">
-        <v>0</v>
-      </c>
-      <c r="N48" t="n">
-        <v>15</v>
-      </c>
-      <c r="O48" t="n">
-        <v>1824</v>
-      </c>
-      <c r="P48" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q48" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="n">
-        <v>44852</v>
-      </c>
-      <c r="B49" t="n">
-        <v>27</v>
-      </c>
-      <c r="C49" t="n">
-        <v>1768</v>
-      </c>
-      <c r="D49" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" t="n">
-        <v>0</v>
-      </c>
-      <c r="F49" t="n">
-        <v>1</v>
-      </c>
-      <c r="G49" t="n">
-        <v>1938.17</v>
-      </c>
-      <c r="H49" t="n">
-        <v>0</v>
-      </c>
-      <c r="I49" t="n">
-        <v>0</v>
-      </c>
-      <c r="J49" t="n">
-        <v>24</v>
-      </c>
-      <c r="K49" t="n">
-        <v>1505</v>
-      </c>
-      <c r="L49" t="n">
-        <v>0</v>
-      </c>
-      <c r="M49" t="n">
-        <v>0</v>
-      </c>
-      <c r="N49" t="n">
-        <v>15</v>
-      </c>
-      <c r="O49" t="n">
-        <v>1824</v>
-      </c>
-      <c r="P49" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q49" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="n">
-        <v>44853</v>
-      </c>
-      <c r="B50" t="n">
-        <v>27</v>
-      </c>
-      <c r="C50" t="n">
-        <v>1768</v>
-      </c>
-      <c r="D50" t="n">
-        <v>0</v>
-      </c>
-      <c r="E50" t="n">
-        <v>0</v>
-      </c>
-      <c r="F50" t="n">
-        <v>1</v>
-      </c>
-      <c r="G50" t="n">
-        <v>1965.65</v>
-      </c>
-      <c r="H50" t="n">
-        <v>0</v>
-      </c>
-      <c r="I50" t="n">
-        <v>0</v>
-      </c>
-      <c r="J50" t="n">
-        <v>21</v>
-      </c>
-      <c r="K50" t="n">
-        <v>1404</v>
-      </c>
-      <c r="L50" t="n">
-        <v>0</v>
-      </c>
-      <c r="M50" t="n">
-        <v>0</v>
-      </c>
-      <c r="N50" t="n">
-        <v>0</v>
-      </c>
-      <c r="O50" t="n">
-        <v>0</v>
-      </c>
-      <c r="P50" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q50" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="n">
-        <v>44854</v>
-      </c>
-      <c r="B51" t="n">
-        <v>25</v>
-      </c>
-      <c r="C51" t="n">
-        <v>1825</v>
-      </c>
-      <c r="D51" t="n">
-        <v>0</v>
-      </c>
-      <c r="E51" t="n">
-        <v>0</v>
-      </c>
-      <c r="F51" t="n">
-        <v>1</v>
-      </c>
-      <c r="G51" t="n">
-        <v>1966</v>
-      </c>
-      <c r="H51" t="n">
-        <v>0</v>
-      </c>
-      <c r="I51" t="n">
-        <v>0</v>
-      </c>
-      <c r="J51" t="n">
-        <v>20</v>
-      </c>
-      <c r="K51" t="n">
-        <v>1404</v>
-      </c>
-      <c r="L51" t="n">
-        <v>0</v>
-      </c>
-      <c r="M51" t="n">
-        <v>0</v>
-      </c>
-      <c r="N51" t="n">
-        <v>0</v>
-      </c>
-      <c r="O51" t="n">
-        <v>0</v>
-      </c>
-      <c r="P51" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q51" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="n">
-        <v>44855</v>
-      </c>
-      <c r="B52" t="n">
-        <v>29</v>
-      </c>
-      <c r="C52" t="n">
-        <v>1725</v>
-      </c>
-      <c r="D52" t="n">
-        <v>0</v>
-      </c>
-      <c r="E52" t="n">
-        <v>0</v>
-      </c>
-      <c r="F52" t="n">
-        <v>1</v>
-      </c>
-      <c r="G52" t="n">
-        <v>1966</v>
-      </c>
-      <c r="H52" t="n">
-        <v>11</v>
-      </c>
-      <c r="I52" t="n">
-        <v>1343.48</v>
-      </c>
-      <c r="J52" t="n">
-        <v>11</v>
-      </c>
-      <c r="K52" t="n">
-        <v>1274.7</v>
-      </c>
-      <c r="L52" t="n">
-        <v>0</v>
-      </c>
-      <c r="M52" t="n">
-        <v>0</v>
-      </c>
-      <c r="N52" t="n">
-        <v>0</v>
-      </c>
-      <c r="O52" t="n">
-        <v>0</v>
-      </c>
-      <c r="P52" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q52" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="1" t="n">
-        <v>44856</v>
-      </c>
-      <c r="B53" t="n">
-        <v>32</v>
-      </c>
-      <c r="C53" t="n">
-        <v>1893</v>
-      </c>
-      <c r="D53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E53" t="n">
-        <v>0</v>
-      </c>
-      <c r="F53" t="n">
-        <v>1</v>
-      </c>
-      <c r="G53" t="n">
-        <v>1982.96</v>
-      </c>
-      <c r="H53" t="n">
-        <v>22</v>
-      </c>
-      <c r="I53" t="n">
-        <v>1654.28</v>
-      </c>
-      <c r="J53" t="n">
-        <v>5</v>
-      </c>
-      <c r="K53" t="n">
-        <v>1509</v>
-      </c>
-      <c r="L53" t="n">
-        <v>0</v>
-      </c>
-      <c r="M53" t="n">
-        <v>0</v>
-      </c>
-      <c r="N53" t="n">
-        <v>0</v>
-      </c>
-      <c r="O53" t="n">
-        <v>0</v>
-      </c>
-      <c r="P53" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q53" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="1" t="n">
-        <v>44857</v>
-      </c>
-      <c r="B54" t="n">
-        <v>25</v>
-      </c>
-      <c r="C54" t="n">
-        <v>1825</v>
-      </c>
-      <c r="D54" t="n">
-        <v>0</v>
-      </c>
-      <c r="E54" t="n">
-        <v>0</v>
-      </c>
-      <c r="F54" t="n">
-        <v>0</v>
-      </c>
-      <c r="G54" t="n">
-        <v>0</v>
-      </c>
-      <c r="H54" t="n">
-        <v>22</v>
-      </c>
-      <c r="I54" t="n">
-        <v>1760.3</v>
-      </c>
-      <c r="J54" t="n">
-        <v>5</v>
-      </c>
-      <c r="K54" t="n">
-        <v>1403.61</v>
-      </c>
-      <c r="L54" t="n">
-        <v>0</v>
-      </c>
-      <c r="M54" t="n">
-        <v>0</v>
-      </c>
-      <c r="N54" t="n">
-        <v>0</v>
-      </c>
-      <c r="O54" t="n">
-        <v>0</v>
-      </c>
-      <c r="P54" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q54" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="1" t="n">
-        <v>44858</v>
-      </c>
-      <c r="B55" t="n">
-        <v>24</v>
-      </c>
-      <c r="C55" t="n">
-        <v>1902.61</v>
-      </c>
-      <c r="D55" t="n">
-        <v>0</v>
-      </c>
-      <c r="E55" t="n">
-        <v>0</v>
-      </c>
-      <c r="F55" t="n">
-        <v>0</v>
-      </c>
-      <c r="G55" t="n">
-        <v>0</v>
-      </c>
-      <c r="H55" t="n">
-        <v>12</v>
-      </c>
-      <c r="I55" t="n">
-        <v>1689.13</v>
-      </c>
-      <c r="J55" t="n">
-        <v>12</v>
-      </c>
-      <c r="K55" t="n">
-        <v>1419.35</v>
-      </c>
-      <c r="L55" t="n">
-        <v>0</v>
-      </c>
-      <c r="M55" t="n">
-        <v>0</v>
-      </c>
-      <c r="N55" t="n">
-        <v>10</v>
-      </c>
-      <c r="O55" t="n">
-        <v>1824</v>
-      </c>
-      <c r="P55" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q55" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="n">
-        <v>44859</v>
-      </c>
-      <c r="B56" t="n">
-        <v>28</v>
-      </c>
-      <c r="C56" t="n">
-        <v>1825</v>
-      </c>
-      <c r="D56" t="n">
-        <v>0</v>
-      </c>
-      <c r="E56" t="n">
-        <v>0</v>
-      </c>
-      <c r="F56" t="n">
-        <v>0</v>
-      </c>
-      <c r="G56" t="n">
-        <v>0</v>
-      </c>
-      <c r="H56" t="n">
-        <v>0</v>
-      </c>
-      <c r="I56" t="n">
-        <v>0</v>
-      </c>
-      <c r="J56" t="n">
-        <v>12</v>
-      </c>
-      <c r="K56" t="n">
-        <v>1527</v>
-      </c>
-      <c r="L56" t="n">
-        <v>0</v>
-      </c>
-      <c r="M56" t="n">
-        <v>0</v>
-      </c>
-      <c r="N56" t="n">
-        <v>10</v>
-      </c>
-      <c r="O56" t="n">
-        <v>1824</v>
-      </c>
-      <c r="P56" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q56" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="1" t="n">
-        <v>44860</v>
-      </c>
-      <c r="B57" t="n">
-        <v>26</v>
-      </c>
-      <c r="C57" t="n">
-        <v>1775.64</v>
-      </c>
-      <c r="D57" t="n">
-        <v>0</v>
-      </c>
-      <c r="E57" t="n">
-        <v>0</v>
-      </c>
-      <c r="F57" t="n">
-        <v>0</v>
-      </c>
-      <c r="G57" t="n">
-        <v>0</v>
-      </c>
-      <c r="H57" t="n">
-        <v>12</v>
-      </c>
-      <c r="I57" t="n">
-        <v>1804.04</v>
-      </c>
-      <c r="J57" t="n">
-        <v>12</v>
-      </c>
-      <c r="K57" t="n">
-        <v>1509.04</v>
-      </c>
-      <c r="L57" t="n">
-        <v>0</v>
-      </c>
-      <c r="M57" t="n">
-        <v>0</v>
-      </c>
-      <c r="N57" t="n">
-        <v>0</v>
-      </c>
-      <c r="O57" t="n">
-        <v>0</v>
-      </c>
-      <c r="P57" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q57" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="1" t="n">
-        <v>44861</v>
-      </c>
-      <c r="B58" t="n">
-        <v>23</v>
-      </c>
-      <c r="C58" t="n">
-        <v>1854</v>
-      </c>
-      <c r="D58" t="n">
-        <v>0</v>
-      </c>
-      <c r="E58" t="n">
-        <v>0</v>
-      </c>
-      <c r="F58" t="n">
-        <v>0</v>
-      </c>
-      <c r="G58" t="n">
-        <v>0</v>
-      </c>
-      <c r="H58" t="n">
-        <v>12</v>
-      </c>
-      <c r="I58" t="n">
-        <v>1804.04</v>
-      </c>
-      <c r="J58" t="n">
-        <v>12</v>
-      </c>
-      <c r="K58" t="n">
-        <v>1480.4</v>
-      </c>
-      <c r="L58" t="n">
-        <v>0</v>
-      </c>
-      <c r="M58" t="n">
-        <v>0</v>
-      </c>
-      <c r="N58" t="n">
-        <v>0</v>
-      </c>
-      <c r="O58" t="n">
-        <v>0</v>
-      </c>
-      <c r="P58" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q58" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="1" t="n">
-        <v>44862</v>
-      </c>
-      <c r="B59" t="n">
-        <v>30</v>
-      </c>
-      <c r="C59" t="n">
-        <v>1854</v>
-      </c>
-      <c r="D59" t="n">
-        <v>0</v>
-      </c>
-      <c r="E59" t="n">
-        <v>0</v>
-      </c>
-      <c r="F59" t="n">
-        <v>0</v>
-      </c>
-      <c r="G59" t="n">
-        <v>0</v>
-      </c>
-      <c r="H59" t="n">
-        <v>11</v>
-      </c>
-      <c r="I59" t="n">
-        <v>1343.48</v>
-      </c>
-      <c r="J59" t="n">
-        <v>12</v>
-      </c>
-      <c r="K59" t="n">
-        <v>1395.65</v>
-      </c>
-      <c r="L59" t="n">
-        <v>0</v>
-      </c>
-      <c r="M59" t="n">
-        <v>0</v>
-      </c>
-      <c r="N59" t="n">
-        <v>0</v>
-      </c>
-      <c r="O59" t="n">
-        <v>0</v>
-      </c>
-      <c r="P59" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q59" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="1" t="n">
-        <v>44863</v>
-      </c>
-      <c r="B60" t="n">
-        <v>32</v>
-      </c>
-      <c r="C60" t="n">
-        <v>1854</v>
-      </c>
-      <c r="D60" t="n">
-        <v>0</v>
-      </c>
-      <c r="E60" t="n">
-        <v>0</v>
-      </c>
-      <c r="F60" t="n">
-        <v>0</v>
-      </c>
-      <c r="G60" t="n">
-        <v>0</v>
-      </c>
-      <c r="H60" t="n">
-        <v>11</v>
-      </c>
-      <c r="I60" t="n">
-        <v>1343.48</v>
-      </c>
-      <c r="J60" t="n">
-        <v>13</v>
-      </c>
-      <c r="K60" t="n">
-        <v>1425</v>
-      </c>
-      <c r="L60" t="n">
-        <v>0</v>
-      </c>
-      <c r="M60" t="n">
-        <v>0</v>
-      </c>
-      <c r="N60" t="n">
-        <v>0</v>
-      </c>
-      <c r="O60" t="n">
-        <v>0</v>
-      </c>
-      <c r="P60" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q60" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="1" t="n">
-        <v>44864</v>
-      </c>
-      <c r="B61" t="n">
-        <v>27</v>
-      </c>
-      <c r="C61" t="n">
-        <v>1803</v>
-      </c>
-      <c r="D61" t="n">
-        <v>0</v>
-      </c>
-      <c r="E61" t="n">
-        <v>0</v>
-      </c>
-      <c r="F61" t="n">
-        <v>1</v>
-      </c>
-      <c r="G61" t="n">
-        <v>1477</v>
-      </c>
-      <c r="H61" t="n">
-        <v>11</v>
-      </c>
-      <c r="I61" t="n">
-        <v>1343.48</v>
-      </c>
-      <c r="J61" t="n">
-        <v>15</v>
-      </c>
-      <c r="K61" t="n">
-        <v>1405.06</v>
-      </c>
-      <c r="L61" t="n">
-        <v>0</v>
-      </c>
-      <c r="M61" t="n">
-        <v>0</v>
-      </c>
-      <c r="N61" t="n">
-        <v>0</v>
-      </c>
-      <c r="O61" t="n">
-        <v>0</v>
-      </c>
-      <c r="P61" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q61" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="1" t="n">
-        <v>44865</v>
-      </c>
-      <c r="B62" t="n">
-        <v>27</v>
-      </c>
-      <c r="C62" t="n">
-        <v>1803.09</v>
-      </c>
-      <c r="D62" t="n">
-        <v>0</v>
-      </c>
-      <c r="E62" t="n">
-        <v>0</v>
-      </c>
-      <c r="F62" t="n">
-        <v>0</v>
-      </c>
-      <c r="G62" t="n">
-        <v>0</v>
-      </c>
-      <c r="H62" t="n">
-        <v>11</v>
-      </c>
-      <c r="I62" t="n">
-        <v>1343.48</v>
-      </c>
-      <c r="J62" t="n">
-        <v>13</v>
-      </c>
-      <c r="K62" t="n">
-        <v>1395.65</v>
-      </c>
-      <c r="L62" t="n">
-        <v>0</v>
-      </c>
-      <c r="M62" t="n">
-        <v>0</v>
-      </c>
-      <c r="N62" t="n">
-        <v>0</v>
-      </c>
-      <c r="O62" t="n">
-        <v>0</v>
-      </c>
-      <c r="P62" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q62" t="n">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Again error with pasting in Excel
</commit_message>
<xml_diff>
--- a/NameFile.xlsx
+++ b/NameFile.xlsx
@@ -3485,46 +3485,46 @@
         <v>0</v>
       </c>
       <c r="R32" t="n">
+        <v>0</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0</v>
+      </c>
+      <c r="T32" t="n">
+        <v>1</v>
+      </c>
+      <c r="U32" t="n">
+        <v>45.92</v>
+      </c>
+      <c r="V32" t="n">
+        <v>0</v>
+      </c>
+      <c r="W32" t="n">
+        <v>0</v>
+      </c>
+      <c r="X32" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>1555.12</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD32" t="n">
         <v>4</v>
       </c>
-      <c r="S32" t="n">
+      <c r="AE32" t="n">
         <v>148.32</v>
-      </c>
-      <c r="T32" t="n">
-        <v>0</v>
-      </c>
-      <c r="U32" t="n">
-        <v>0</v>
-      </c>
-      <c r="V32" t="n">
-        <v>1</v>
-      </c>
-      <c r="W32" t="n">
-        <v>45.92</v>
-      </c>
-      <c r="X32" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y32" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB32" t="n">
-        <v>14</v>
-      </c>
-      <c r="AC32" t="n">
-        <v>1555.12</v>
-      </c>
-      <c r="AD32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE32" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -3550,58 +3550,58 @@
         <v>313.06</v>
       </c>
       <c r="H33" t="n">
+        <v>1</v>
+      </c>
+      <c r="I33" t="n">
+        <v>-12.5</v>
+      </c>
+      <c r="J33" t="n">
         <v>2</v>
       </c>
-      <c r="I33" t="n">
+      <c r="K33" t="n">
         <v>352.92</v>
       </c>
-      <c r="J33" t="n">
-        <v>0</v>
-      </c>
-      <c r="K33" t="n">
-        <v>0</v>
-      </c>
       <c r="L33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" t="n">
+        <v>1</v>
+      </c>
+      <c r="O33" t="n">
         <v>107.33</v>
       </c>
-      <c r="N33" t="n">
-        <v>1</v>
-      </c>
-      <c r="O33" t="n">
-        <v>0</v>
-      </c>
       <c r="P33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q33" t="n">
-        <v>-12.5</v>
+        <v>0</v>
       </c>
       <c r="R33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S33" t="n">
         <v>0</v>
       </c>
       <c r="T33" t="n">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="U33" t="n">
-        <v>0</v>
+        <v>4284.28</v>
       </c>
       <c r="V33" t="n">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="W33" t="n">
-        <v>4284.28</v>
+        <v>0</v>
       </c>
       <c r="X33" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Y33" t="n">
-        <v>0</v>
+        <v>403.68</v>
       </c>
       <c r="Z33" t="n">
         <v>0</v>
@@ -3610,13 +3610,13 @@
         <v>0</v>
       </c>
       <c r="AB33" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AC33" t="n">
-        <v>403.68</v>
+        <v>0</v>
       </c>
       <c r="AD33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE33" t="n">
         <v>0</v>
@@ -3645,17 +3645,17 @@
         <v>348.78</v>
       </c>
       <c r="H34" t="n">
+        <v>3</v>
+      </c>
+      <c r="I34" t="n">
+        <v>133.32</v>
+      </c>
+      <c r="J34" t="n">
         <v>4</v>
       </c>
-      <c r="I34" t="n">
+      <c r="K34" t="n">
         <v>626.24</v>
       </c>
-      <c r="J34" t="n">
-        <v>0</v>
-      </c>
-      <c r="K34" t="n">
-        <v>0</v>
-      </c>
       <c r="L34" t="n">
         <v>0</v>
       </c>
@@ -3669,13 +3669,13 @@
         <v>0</v>
       </c>
       <c r="P34" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q34" t="n">
-        <v>133.32</v>
+        <v>0</v>
       </c>
       <c r="R34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S34" t="n">
         <v>0</v>
@@ -3693,10 +3693,10 @@
         <v>0</v>
       </c>
       <c r="X34" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Y34" t="n">
-        <v>0</v>
+        <v>-364.2</v>
       </c>
       <c r="Z34" t="n">
         <v>0</v>
@@ -3705,13 +3705,13 @@
         <v>0</v>
       </c>
       <c r="AB34" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AC34" t="n">
-        <v>-364.2</v>
+        <v>0</v>
       </c>
       <c r="AD34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE34" t="n">
         <v>0</v>
@@ -3740,7 +3740,7 @@
         <v>294.74</v>
       </c>
       <c r="H35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35" t="n">
         <v>0</v>
@@ -3758,58 +3758,58 @@
         <v>0</v>
       </c>
       <c r="N35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O35" t="n">
         <v>0</v>
       </c>
       <c r="P35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q35" t="n">
         <v>0</v>
       </c>
       <c r="R35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S35" t="n">
+        <v>0</v>
+      </c>
+      <c r="T35" t="n">
+        <v>12</v>
+      </c>
+      <c r="U35" t="n">
+        <v>2000.64</v>
+      </c>
+      <c r="V35" t="n">
+        <v>0</v>
+      </c>
+      <c r="W35" t="n">
+        <v>0</v>
+      </c>
+      <c r="X35" t="n">
+        <v>25</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>3508</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE35" t="n">
         <v>83.33</v>
-      </c>
-      <c r="T35" t="n">
-        <v>0</v>
-      </c>
-      <c r="U35" t="n">
-        <v>0</v>
-      </c>
-      <c r="V35" t="n">
-        <v>12</v>
-      </c>
-      <c r="W35" t="n">
-        <v>2000.64</v>
-      </c>
-      <c r="X35" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y35" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB35" t="n">
-        <v>25</v>
-      </c>
-      <c r="AC35" t="n">
-        <v>3508</v>
-      </c>
-      <c r="AD35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE35" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -3835,7 +3835,7 @@
         <v>0</v>
       </c>
       <c r="H36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36" t="n">
         <v>0</v>
@@ -3847,46 +3847,46 @@
         <v>0</v>
       </c>
       <c r="L36" t="n">
+        <v>0</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0</v>
+      </c>
+      <c r="N36" t="n">
         <v>2</v>
       </c>
-      <c r="M36" t="n">
+      <c r="O36" t="n">
         <v>136.26</v>
       </c>
-      <c r="N36" t="n">
-        <v>0</v>
-      </c>
-      <c r="O36" t="n">
-        <v>0</v>
-      </c>
       <c r="P36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q36" t="n">
         <v>0</v>
       </c>
       <c r="R36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S36" t="n">
         <v>0</v>
       </c>
       <c r="T36" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U36" t="n">
-        <v>0</v>
+        <v>192.12</v>
       </c>
       <c r="V36" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="W36" t="n">
-        <v>192.12</v>
+        <v>0</v>
       </c>
       <c r="X36" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="Y36" t="n">
-        <v>0</v>
+        <v>2634.06</v>
       </c>
       <c r="Z36" t="n">
         <v>0</v>
@@ -3895,13 +3895,13 @@
         <v>0</v>
       </c>
       <c r="AB36" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="AC36" t="n">
-        <v>2634.06</v>
+        <v>0</v>
       </c>
       <c r="AD36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE36" t="n">
         <v>0</v>
@@ -3930,58 +3930,58 @@
         <v>336.9</v>
       </c>
       <c r="H37" t="n">
+        <v>1</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="n">
         <v>2</v>
       </c>
-      <c r="I37" t="n">
+      <c r="K37" t="n">
         <v>170</v>
       </c>
-      <c r="J37" t="n">
-        <v>0</v>
-      </c>
-      <c r="K37" t="n">
-        <v>0</v>
-      </c>
       <c r="L37" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" t="n">
         <v>6</v>
       </c>
-      <c r="M37" t="n">
+      <c r="O37" t="n">
         <v>402.48</v>
       </c>
-      <c r="N37" t="n">
-        <v>0</v>
-      </c>
-      <c r="O37" t="n">
-        <v>0</v>
-      </c>
       <c r="P37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q37" t="n">
         <v>0</v>
       </c>
       <c r="R37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S37" t="n">
         <v>0</v>
       </c>
       <c r="T37" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U37" t="n">
-        <v>0</v>
+        <v>301.12</v>
       </c>
       <c r="V37" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W37" t="n">
-        <v>301.12</v>
+        <v>0</v>
       </c>
       <c r="X37" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Y37" t="n">
-        <v>0</v>
+        <v>1012.92</v>
       </c>
       <c r="Z37" t="n">
         <v>0</v>
@@ -3990,13 +3990,13 @@
         <v>0</v>
       </c>
       <c r="AB37" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AC37" t="n">
-        <v>1012.92</v>
+        <v>0</v>
       </c>
       <c r="AD37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE37" t="n">
         <v>0</v>
@@ -4028,73 +4028,73 @@
         <v>1</v>
       </c>
       <c r="I38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="n">
+        <v>1</v>
+      </c>
+      <c r="K38" t="n">
         <v>110.5</v>
       </c>
-      <c r="J38" t="n">
-        <v>0</v>
-      </c>
-      <c r="K38" t="n">
-        <v>0</v>
-      </c>
       <c r="L38" t="n">
+        <v>0</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0</v>
+      </c>
+      <c r="N38" t="n">
         <v>5</v>
       </c>
-      <c r="M38" t="n">
+      <c r="O38" t="n">
         <v>492.9</v>
       </c>
-      <c r="N38" t="n">
-        <v>0</v>
-      </c>
-      <c r="O38" t="n">
-        <v>0</v>
-      </c>
       <c r="P38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q38" t="n">
         <v>0</v>
       </c>
       <c r="R38" t="n">
+        <v>0</v>
+      </c>
+      <c r="S38" t="n">
+        <v>0</v>
+      </c>
+      <c r="T38" t="n">
+        <v>20</v>
+      </c>
+      <c r="U38" t="n">
+        <v>1727.4</v>
+      </c>
+      <c r="V38" t="n">
+        <v>0</v>
+      </c>
+      <c r="W38" t="n">
+        <v>0</v>
+      </c>
+      <c r="X38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y38" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD38" t="n">
         <v>2</v>
       </c>
-      <c r="S38" t="n">
+      <c r="AE38" t="n">
         <v>85</v>
-      </c>
-      <c r="T38" t="n">
-        <v>0</v>
-      </c>
-      <c r="U38" t="n">
-        <v>0</v>
-      </c>
-      <c r="V38" t="n">
-        <v>20</v>
-      </c>
-      <c r="W38" t="n">
-        <v>1727.4</v>
-      </c>
-      <c r="X38" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y38" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE38" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -4120,76 +4120,76 @@
         <v>356.72</v>
       </c>
       <c r="H39" t="n">
+        <v>1</v>
+      </c>
+      <c r="I39" t="n">
+        <v>0</v>
+      </c>
+      <c r="J39" t="n">
         <v>8</v>
       </c>
-      <c r="I39" t="n">
+      <c r="K39" t="n">
         <v>612.16</v>
       </c>
-      <c r="J39" t="n">
-        <v>0</v>
-      </c>
-      <c r="K39" t="n">
-        <v>0</v>
-      </c>
       <c r="L39" t="n">
+        <v>0</v>
+      </c>
+      <c r="M39" t="n">
+        <v>0</v>
+      </c>
+      <c r="N39" t="n">
         <v>4</v>
       </c>
-      <c r="M39" t="n">
+      <c r="O39" t="n">
         <v>386.84</v>
       </c>
-      <c r="N39" t="n">
-        <v>0</v>
-      </c>
-      <c r="O39" t="n">
-        <v>0</v>
-      </c>
       <c r="P39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q39" t="n">
         <v>0</v>
       </c>
       <c r="R39" t="n">
+        <v>0</v>
+      </c>
+      <c r="S39" t="n">
+        <v>0</v>
+      </c>
+      <c r="T39" t="n">
+        <v>11</v>
+      </c>
+      <c r="U39" t="n">
+        <v>999.5700000000001</v>
+      </c>
+      <c r="V39" t="n">
+        <v>0</v>
+      </c>
+      <c r="W39" t="n">
+        <v>0</v>
+      </c>
+      <c r="X39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y39" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD39" t="n">
         <v>3</v>
       </c>
-      <c r="S39" t="n">
+      <c r="AE39" t="n">
         <v>199.74</v>
-      </c>
-      <c r="T39" t="n">
-        <v>0</v>
-      </c>
-      <c r="U39" t="n">
-        <v>0</v>
-      </c>
-      <c r="V39" t="n">
-        <v>11</v>
-      </c>
-      <c r="W39" t="n">
-        <v>999.5700000000001</v>
-      </c>
-      <c r="X39" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y39" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE39" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -4215,17 +4215,17 @@
         <v>447.3</v>
       </c>
       <c r="H40" t="n">
+        <v>1</v>
+      </c>
+      <c r="I40" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" t="n">
         <v>2</v>
       </c>
-      <c r="I40" t="n">
+      <c r="K40" t="n">
         <v>131.54</v>
       </c>
-      <c r="J40" t="n">
-        <v>0</v>
-      </c>
-      <c r="K40" t="n">
-        <v>0</v>
-      </c>
       <c r="L40" t="n">
         <v>0</v>
       </c>
@@ -4239,28 +4239,28 @@
         <v>0</v>
       </c>
       <c r="P40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q40" t="n">
         <v>0</v>
       </c>
       <c r="R40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S40" t="n">
         <v>0</v>
       </c>
       <c r="T40" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U40" t="n">
-        <v>0</v>
+        <v>298.32</v>
       </c>
       <c r="V40" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="W40" t="n">
-        <v>298.32</v>
+        <v>1115.82</v>
       </c>
       <c r="X40" t="n">
         <v>0</v>
@@ -4269,10 +4269,10 @@
         <v>0</v>
       </c>
       <c r="Z40" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AA40" t="n">
-        <v>1115.82</v>
+        <v>0</v>
       </c>
       <c r="AB40" t="n">
         <v>0</v>
@@ -4281,7 +4281,7 @@
         <v>0</v>
       </c>
       <c r="AD40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE40" t="n">
         <v>0</v>
@@ -4310,7 +4310,7 @@
         <v>551.4000000000001</v>
       </c>
       <c r="H41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41" t="n">
         <v>0</v>
@@ -4334,49 +4334,49 @@
         <v>0</v>
       </c>
       <c r="P41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q41" t="n">
         <v>0</v>
       </c>
       <c r="R41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S41" t="n">
         <v>0</v>
       </c>
       <c r="T41" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U41" t="n">
-        <v>0</v>
+        <v>312.5</v>
       </c>
       <c r="V41" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="W41" t="n">
-        <v>312.5</v>
+        <v>778.3200000000001</v>
       </c>
       <c r="X41" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Y41" t="n">
-        <v>0</v>
+        <v>1146.48</v>
       </c>
       <c r="Z41" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AA41" t="n">
-        <v>778.3200000000001</v>
+        <v>0</v>
       </c>
       <c r="AB41" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AC41" t="n">
-        <v>1146.48</v>
+        <v>0</v>
       </c>
       <c r="AD41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE41" t="n">
         <v>0</v>
@@ -4405,7 +4405,7 @@
         <v>135.67</v>
       </c>
       <c r="H42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42" t="n">
         <v>0</v>
@@ -4429,49 +4429,49 @@
         <v>0</v>
       </c>
       <c r="P42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q42" t="n">
         <v>0</v>
       </c>
       <c r="R42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S42" t="n">
         <v>0</v>
       </c>
       <c r="T42" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="U42" t="n">
-        <v>0</v>
+        <v>2327.04</v>
       </c>
       <c r="V42" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="W42" t="n">
-        <v>2327.04</v>
+        <v>1003.32</v>
       </c>
       <c r="X42" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Y42" t="n">
-        <v>0</v>
+        <v>1505.1</v>
       </c>
       <c r="Z42" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AA42" t="n">
-        <v>1003.32</v>
+        <v>0</v>
       </c>
       <c r="AB42" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AC42" t="n">
-        <v>1505.1</v>
+        <v>0</v>
       </c>
       <c r="AD42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE42" t="n">
         <v>0</v>
@@ -4500,7 +4500,7 @@
         <v>0</v>
       </c>
       <c r="H43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43" t="n">
         <v>0</v>
@@ -4524,34 +4524,34 @@
         <v>0</v>
       </c>
       <c r="P43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q43" t="n">
         <v>0</v>
       </c>
       <c r="R43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S43" t="n">
         <v>0</v>
       </c>
       <c r="T43" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U43" t="n">
-        <v>0</v>
+        <v>298.32</v>
       </c>
       <c r="V43" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W43" t="n">
-        <v>298.32</v>
+        <v>0</v>
       </c>
       <c r="X43" t="n">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="Y43" t="n">
-        <v>0</v>
+        <v>5266.52</v>
       </c>
       <c r="Z43" t="n">
         <v>0</v>
@@ -4560,13 +4560,13 @@
         <v>0</v>
       </c>
       <c r="AB43" t="n">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="AC43" t="n">
-        <v>5266.52</v>
+        <v>0</v>
       </c>
       <c r="AD43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE43" t="n">
         <v>0</v>
@@ -4595,10 +4595,10 @@
         <v>109.5</v>
       </c>
       <c r="H44" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="J44" t="n">
         <v>0</v>
@@ -4619,28 +4619,28 @@
         <v>0</v>
       </c>
       <c r="P44" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q44" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="R44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S44" t="n">
         <v>0</v>
       </c>
       <c r="T44" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="U44" t="n">
-        <v>0</v>
+        <v>1742.11</v>
       </c>
       <c r="V44" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="W44" t="n">
-        <v>1742.11</v>
+        <v>0</v>
       </c>
       <c r="X44" t="n">
         <v>0</v>
@@ -4661,7 +4661,7 @@
         <v>0</v>
       </c>
       <c r="AD44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE44" t="n">
         <v>0</v>
@@ -4690,7 +4690,7 @@
         <v>264.9</v>
       </c>
       <c r="H45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45" t="n">
         <v>0</v>
@@ -4714,28 +4714,28 @@
         <v>0</v>
       </c>
       <c r="P45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q45" t="n">
         <v>0</v>
       </c>
       <c r="R45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S45" t="n">
         <v>0</v>
       </c>
       <c r="T45" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U45" t="n">
-        <v>0</v>
+        <v>298.32</v>
       </c>
       <c r="V45" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W45" t="n">
-        <v>298.32</v>
+        <v>0</v>
       </c>
       <c r="X45" t="n">
         <v>0</v>
@@ -4756,7 +4756,7 @@
         <v>0</v>
       </c>
       <c r="AD45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE45" t="n">
         <v>0</v>
@@ -4785,7 +4785,7 @@
         <v>415</v>
       </c>
       <c r="H46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I46" t="n">
         <v>0</v>
@@ -4809,34 +4809,34 @@
         <v>0</v>
       </c>
       <c r="P46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q46" t="n">
         <v>0</v>
       </c>
       <c r="R46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S46" t="n">
         <v>0</v>
       </c>
       <c r="T46" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="U46" t="n">
-        <v>0</v>
+        <v>1229.49</v>
       </c>
       <c r="V46" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="W46" t="n">
-        <v>1229.49</v>
+        <v>0</v>
       </c>
       <c r="X46" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y46" t="n">
-        <v>0</v>
+        <v>187.5</v>
       </c>
       <c r="Z46" t="n">
         <v>0</v>
@@ -4845,13 +4845,13 @@
         <v>0</v>
       </c>
       <c r="AB46" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC46" t="n">
-        <v>187.5</v>
+        <v>0</v>
       </c>
       <c r="AD46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE46" t="n">
         <v>0</v>
@@ -4880,7 +4880,7 @@
         <v>397.08</v>
       </c>
       <c r="H47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I47" t="n">
         <v>0</v>
@@ -4904,28 +4904,28 @@
         <v>0</v>
       </c>
       <c r="P47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q47" t="n">
         <v>0</v>
       </c>
       <c r="R47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S47" t="n">
         <v>0</v>
       </c>
       <c r="T47" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="U47" t="n">
-        <v>0</v>
+        <v>1717</v>
       </c>
       <c r="V47" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="W47" t="n">
-        <v>1717</v>
+        <v>0</v>
       </c>
       <c r="X47" t="n">
         <v>0</v>
@@ -4946,7 +4946,7 @@
         <v>0</v>
       </c>
       <c r="AD47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE47" t="n">
         <v>0</v>
@@ -4975,7 +4975,7 @@
         <v>716.0999999999999</v>
       </c>
       <c r="H48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I48" t="n">
         <v>0</v>
@@ -4999,34 +4999,34 @@
         <v>0</v>
       </c>
       <c r="P48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q48" t="n">
         <v>0</v>
       </c>
       <c r="R48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S48" t="n">
         <v>0</v>
       </c>
       <c r="T48" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="U48" t="n">
-        <v>0</v>
+        <v>1099.12</v>
       </c>
       <c r="V48" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="W48" t="n">
-        <v>1099.12</v>
+        <v>0</v>
       </c>
       <c r="X48" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Y48" t="n">
-        <v>0</v>
+        <v>956.6799999999999</v>
       </c>
       <c r="Z48" t="n">
         <v>0</v>
@@ -5035,13 +5035,13 @@
         <v>0</v>
       </c>
       <c r="AB48" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AC48" t="n">
-        <v>956.6799999999999</v>
+        <v>0</v>
       </c>
       <c r="AD48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE48" t="n">
         <v>0</v>
@@ -5070,17 +5070,17 @@
         <v>728.58</v>
       </c>
       <c r="H49" t="n">
+        <v>3</v>
+      </c>
+      <c r="I49" t="n">
+        <v>99.98999999999999</v>
+      </c>
+      <c r="J49" t="n">
         <v>2</v>
       </c>
-      <c r="I49" t="n">
+      <c r="K49" t="n">
         <v>495</v>
       </c>
-      <c r="J49" t="n">
-        <v>0</v>
-      </c>
-      <c r="K49" t="n">
-        <v>0</v>
-      </c>
       <c r="L49" t="n">
         <v>0</v>
       </c>
@@ -5088,40 +5088,40 @@
         <v>0</v>
       </c>
       <c r="N49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O49" t="n">
         <v>0</v>
       </c>
       <c r="P49" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q49" t="n">
-        <v>99.98999999999999</v>
+        <v>0</v>
       </c>
       <c r="R49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S49" t="n">
         <v>0</v>
       </c>
       <c r="T49" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U49" t="n">
-        <v>0</v>
+        <v>1857.12</v>
       </c>
       <c r="V49" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="W49" t="n">
-        <v>1857.12</v>
+        <v>0</v>
       </c>
       <c r="X49" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="Y49" t="n">
-        <v>0</v>
+        <v>1997.27</v>
       </c>
       <c r="Z49" t="n">
         <v>0</v>
@@ -5130,13 +5130,13 @@
         <v>0</v>
       </c>
       <c r="AB49" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="AC49" t="n">
-        <v>1997.27</v>
+        <v>0</v>
       </c>
       <c r="AD49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE49" t="n">
         <v>0</v>
@@ -5165,7 +5165,7 @@
         <v>66.83</v>
       </c>
       <c r="H50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50" t="n">
         <v>0</v>
@@ -5189,46 +5189,46 @@
         <v>0</v>
       </c>
       <c r="P50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q50" t="n">
         <v>0</v>
       </c>
       <c r="R50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S50" t="n">
         <v>0</v>
       </c>
       <c r="T50" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U50" t="n">
-        <v>0</v>
+        <v>298.32</v>
       </c>
       <c r="V50" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W50" t="n">
-        <v>298.32</v>
+        <v>0</v>
       </c>
       <c r="X50" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="Y50" t="n">
-        <v>0</v>
+        <v>1893.6</v>
       </c>
       <c r="Z50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA50" t="n">
         <v>0</v>
       </c>
       <c r="AB50" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="AC50" t="n">
-        <v>1893.6</v>
+        <v>0</v>
       </c>
       <c r="AD50" t="n">
         <v>1</v>
@@ -5260,7 +5260,7 @@
         <v>4.17</v>
       </c>
       <c r="H51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I51" t="n">
         <v>0</v>
@@ -5284,46 +5284,46 @@
         <v>0</v>
       </c>
       <c r="P51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q51" t="n">
         <v>0</v>
       </c>
       <c r="R51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S51" t="n">
         <v>0</v>
       </c>
       <c r="T51" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U51" t="n">
-        <v>0</v>
+        <v>569.16</v>
       </c>
       <c r="V51" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="W51" t="n">
-        <v>569.16</v>
+        <v>0</v>
       </c>
       <c r="X51" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="Y51" t="n">
-        <v>0</v>
+        <v>3705.2</v>
       </c>
       <c r="Z51" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA51" t="n">
         <v>0</v>
       </c>
       <c r="AB51" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AC51" t="n">
-        <v>3705.2</v>
+        <v>0</v>
       </c>
       <c r="AD51" t="n">
         <v>1</v>
@@ -5358,14 +5358,14 @@
         <v>1</v>
       </c>
       <c r="I52" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" t="n">
+        <v>1</v>
+      </c>
+      <c r="K52" t="n">
         <v>110.17</v>
       </c>
-      <c r="J52" t="n">
-        <v>0</v>
-      </c>
-      <c r="K52" t="n">
-        <v>0</v>
-      </c>
       <c r="L52" t="n">
         <v>0</v>
       </c>
@@ -5379,46 +5379,46 @@
         <v>0</v>
       </c>
       <c r="P52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q52" t="n">
         <v>0</v>
       </c>
       <c r="R52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S52" t="n">
         <v>0</v>
       </c>
       <c r="T52" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="U52" t="n">
-        <v>0</v>
+        <v>6195.84</v>
       </c>
       <c r="V52" t="n">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="W52" t="n">
-        <v>6195.84</v>
+        <v>0</v>
       </c>
       <c r="X52" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="Y52" t="n">
-        <v>0</v>
+        <v>3557.6</v>
       </c>
       <c r="Z52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA52" t="n">
         <v>0</v>
       </c>
       <c r="AB52" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AC52" t="n">
-        <v>3557.6</v>
+        <v>0</v>
       </c>
       <c r="AD52" t="n">
         <v>1</v>
@@ -5450,7 +5450,7 @@
         <v>93.79000000000001</v>
       </c>
       <c r="H53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I53" t="n">
         <v>0</v>
@@ -5462,58 +5462,58 @@
         <v>0</v>
       </c>
       <c r="L53" t="n">
+        <v>0</v>
+      </c>
+      <c r="M53" t="n">
+        <v>0</v>
+      </c>
+      <c r="N53" t="n">
         <v>2</v>
       </c>
-      <c r="M53" t="n">
+      <c r="O53" t="n">
         <v>135.84</v>
       </c>
-      <c r="N53" t="n">
-        <v>0</v>
-      </c>
-      <c r="O53" t="n">
-        <v>0</v>
-      </c>
       <c r="P53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q53" t="n">
         <v>0</v>
       </c>
       <c r="R53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S53" t="n">
         <v>0</v>
       </c>
       <c r="T53" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U53" t="n">
-        <v>0</v>
+        <v>372.9</v>
       </c>
       <c r="V53" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="W53" t="n">
-        <v>372.9</v>
+        <v>0</v>
       </c>
       <c r="X53" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="Y53" t="n">
-        <v>0</v>
+        <v>3944.39</v>
       </c>
       <c r="Z53" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA53" t="n">
         <v>0</v>
       </c>
       <c r="AB53" t="n">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="AC53" t="n">
-        <v>3944.39</v>
+        <v>0</v>
       </c>
       <c r="AD53" t="n">
         <v>1</v>
@@ -5545,7 +5545,7 @@
         <v>251.94</v>
       </c>
       <c r="H54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I54" t="n">
         <v>0</v>
@@ -5569,13 +5569,13 @@
         <v>0</v>
       </c>
       <c r="P54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q54" t="n">
         <v>0</v>
       </c>
       <c r="R54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S54" t="n">
         <v>0</v>
@@ -5593,22 +5593,22 @@
         <v>0</v>
       </c>
       <c r="X54" t="n">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="Y54" t="n">
-        <v>0</v>
+        <v>5155.08</v>
       </c>
       <c r="Z54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA54" t="n">
         <v>0</v>
       </c>
       <c r="AB54" t="n">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="AC54" t="n">
-        <v>5155.08</v>
+        <v>0</v>
       </c>
       <c r="AD54" t="n">
         <v>1</v>
@@ -5643,14 +5643,14 @@
         <v>1</v>
       </c>
       <c r="I55" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" t="n">
+        <v>1</v>
+      </c>
+      <c r="K55" t="n">
         <v>160.83</v>
       </c>
-      <c r="J55" t="n">
-        <v>0</v>
-      </c>
-      <c r="K55" t="n">
-        <v>0</v>
-      </c>
       <c r="L55" t="n">
         <v>0</v>
       </c>
@@ -5664,46 +5664,46 @@
         <v>0</v>
       </c>
       <c r="P55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q55" t="n">
         <v>0</v>
       </c>
       <c r="R55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S55" t="n">
         <v>0</v>
       </c>
       <c r="T55" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U55" t="n">
-        <v>0</v>
+        <v>204.16</v>
       </c>
       <c r="V55" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W55" t="n">
-        <v>204.16</v>
+        <v>0</v>
       </c>
       <c r="X55" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Y55" t="n">
-        <v>0</v>
+        <v>955.6400000000001</v>
       </c>
       <c r="Z55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA55" t="n">
         <v>0</v>
       </c>
       <c r="AB55" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AC55" t="n">
-        <v>955.6400000000001</v>
+        <v>0</v>
       </c>
       <c r="AD55" t="n">
         <v>1</v>
@@ -5738,14 +5738,14 @@
         <v>1</v>
       </c>
       <c r="I56" t="n">
+        <v>0</v>
+      </c>
+      <c r="J56" t="n">
+        <v>1</v>
+      </c>
+      <c r="K56" t="n">
         <v>199.17</v>
       </c>
-      <c r="J56" t="n">
-        <v>0</v>
-      </c>
-      <c r="K56" t="n">
-        <v>0</v>
-      </c>
       <c r="L56" t="n">
         <v>0</v>
       </c>
@@ -5759,46 +5759,46 @@
         <v>0</v>
       </c>
       <c r="P56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q56" t="n">
         <v>0</v>
       </c>
       <c r="R56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S56" t="n">
         <v>0</v>
       </c>
       <c r="T56" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U56" t="n">
-        <v>0</v>
+        <v>120.84</v>
       </c>
       <c r="V56" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W56" t="n">
-        <v>120.84</v>
+        <v>0</v>
       </c>
       <c r="X56" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Y56" t="n">
-        <v>0</v>
+        <v>1180.62</v>
       </c>
       <c r="Z56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA56" t="n">
         <v>0</v>
       </c>
       <c r="AB56" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AC56" t="n">
-        <v>1180.62</v>
+        <v>0</v>
       </c>
       <c r="AD56" t="n">
         <v>1</v>
@@ -5830,17 +5830,17 @@
         <v>178.6</v>
       </c>
       <c r="H57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I57" t="n">
+        <v>0</v>
+      </c>
+      <c r="J57" t="n">
+        <v>1</v>
+      </c>
+      <c r="K57" t="n">
         <v>119.17</v>
       </c>
-      <c r="J57" t="n">
-        <v>0</v>
-      </c>
-      <c r="K57" t="n">
-        <v>0</v>
-      </c>
       <c r="L57" t="n">
         <v>0</v>
       </c>
@@ -5860,7 +5860,7 @@
         <v>0</v>
       </c>
       <c r="R57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S57" t="n">
         <v>0</v>
@@ -5878,22 +5878,22 @@
         <v>0</v>
       </c>
       <c r="X57" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="Y57" t="n">
-        <v>0</v>
+        <v>3006</v>
       </c>
       <c r="Z57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA57" t="n">
         <v>0</v>
       </c>
       <c r="AB57" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="AC57" t="n">
-        <v>3006</v>
+        <v>0</v>
       </c>
       <c r="AD57" t="n">
         <v>1</v>
@@ -5955,40 +5955,40 @@
         <v>0</v>
       </c>
       <c r="R58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S58" t="n">
         <v>0</v>
       </c>
       <c r="T58" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="U58" t="n">
-        <v>0</v>
+        <v>1169.63</v>
       </c>
       <c r="V58" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="W58" t="n">
-        <v>1169.63</v>
+        <v>0</v>
       </c>
       <c r="X58" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Y58" t="n">
-        <v>0</v>
+        <v>795.8</v>
       </c>
       <c r="Z58" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA58" t="n">
         <v>0</v>
       </c>
       <c r="AB58" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AC58" t="n">
-        <v>795.8</v>
+        <v>0</v>
       </c>
       <c r="AD58" t="n">
         <v>1</v>
@@ -6020,23 +6020,23 @@
         <v>0</v>
       </c>
       <c r="H59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I59" t="n">
-        <v>0</v>
+        <v>-42.5</v>
       </c>
       <c r="J59" t="n">
+        <v>0</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0</v>
+      </c>
+      <c r="L59" t="n">
         <v>2</v>
       </c>
-      <c r="K59" t="n">
+      <c r="M59" t="n">
         <v>370.84</v>
       </c>
-      <c r="L59" t="n">
-        <v>0</v>
-      </c>
-      <c r="M59" t="n">
-        <v>0</v>
-      </c>
       <c r="N59" t="n">
         <v>0</v>
       </c>
@@ -6044,46 +6044,46 @@
         <v>0</v>
       </c>
       <c r="P59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q59" t="n">
-        <v>-42.5</v>
+        <v>0</v>
       </c>
       <c r="R59" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S59" t="n">
         <v>0</v>
       </c>
       <c r="T59" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="U59" t="n">
-        <v>0</v>
+        <v>7718.9</v>
       </c>
       <c r="V59" t="n">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="W59" t="n">
-        <v>7718.9</v>
+        <v>0</v>
       </c>
       <c r="X59" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Y59" t="n">
-        <v>0</v>
+        <v>795.8</v>
       </c>
       <c r="Z59" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA59" t="n">
         <v>0</v>
       </c>
       <c r="AB59" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AC59" t="n">
-        <v>795.8</v>
+        <v>0</v>
       </c>
       <c r="AD59" t="n">
         <v>1</v>
@@ -6121,23 +6121,23 @@
         <v>0</v>
       </c>
       <c r="J60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K60" t="n">
+        <v>0</v>
+      </c>
+      <c r="L60" t="n">
+        <v>1</v>
+      </c>
+      <c r="M60" t="n">
         <v>62.5</v>
       </c>
-      <c r="L60" t="n">
+      <c r="N60" t="n">
         <v>4</v>
       </c>
-      <c r="M60" t="n">
+      <c r="O60" t="n">
         <v>456.32</v>
       </c>
-      <c r="N60" t="n">
-        <v>0</v>
-      </c>
-      <c r="O60" t="n">
-        <v>0</v>
-      </c>
       <c r="P60" t="n">
         <v>0</v>
       </c>
@@ -6145,22 +6145,22 @@
         <v>0</v>
       </c>
       <c r="R60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S60" t="n">
         <v>0</v>
       </c>
       <c r="T60" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="U60" t="n">
-        <v>0</v>
+        <v>6157.44</v>
       </c>
       <c r="V60" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="W60" t="n">
-        <v>6157.44</v>
+        <v>0</v>
       </c>
       <c r="X60" t="n">
         <v>0</v>
@@ -6169,7 +6169,7 @@
         <v>0</v>
       </c>
       <c r="Z60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA60" t="n">
         <v>0</v>
@@ -6210,23 +6210,23 @@
         <v>122.16</v>
       </c>
       <c r="H61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" t="n">
+        <v>1</v>
+      </c>
+      <c r="K61" t="n">
         <v>136.83</v>
       </c>
-      <c r="J61" t="n">
-        <v>1</v>
-      </c>
-      <c r="K61" t="n">
+      <c r="L61" t="n">
+        <v>1</v>
+      </c>
+      <c r="M61" t="n">
         <v>62.5</v>
       </c>
-      <c r="L61" t="n">
-        <v>0</v>
-      </c>
-      <c r="M61" t="n">
-        <v>0</v>
-      </c>
       <c r="N61" t="n">
         <v>0</v>
       </c>
@@ -6240,40 +6240,40 @@
         <v>0</v>
       </c>
       <c r="R61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S61" t="n">
         <v>0</v>
       </c>
       <c r="T61" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="U61" t="n">
-        <v>0</v>
+        <v>1489.56</v>
       </c>
       <c r="V61" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="W61" t="n">
-        <v>1489.56</v>
+        <v>0</v>
       </c>
       <c r="X61" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y61" t="n">
-        <v>0</v>
+        <v>214.8</v>
       </c>
       <c r="Z61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA61" t="n">
         <v>0</v>
       </c>
       <c r="AB61" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC61" t="n">
-        <v>214.8</v>
+        <v>0</v>
       </c>
       <c r="AD61" t="n">
         <v>1</v>
@@ -6305,17 +6305,17 @@
         <v>162.24</v>
       </c>
       <c r="H62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I62" t="n">
+        <v>0</v>
+      </c>
+      <c r="J62" t="n">
+        <v>1</v>
+      </c>
+      <c r="K62" t="n">
         <v>155.5</v>
       </c>
-      <c r="J62" t="n">
-        <v>0</v>
-      </c>
-      <c r="K62" t="n">
-        <v>0</v>
-      </c>
       <c r="L62" t="n">
         <v>0</v>
       </c>
@@ -6335,40 +6335,40 @@
         <v>0</v>
       </c>
       <c r="R62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S62" t="n">
         <v>0</v>
       </c>
       <c r="T62" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U62" t="n">
-        <v>0</v>
+        <v>510</v>
       </c>
       <c r="V62" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="W62" t="n">
-        <v>510</v>
+        <v>0</v>
       </c>
       <c r="X62" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Y62" t="n">
-        <v>0</v>
+        <v>1419.8</v>
       </c>
       <c r="Z62" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA62" t="n">
         <v>0</v>
       </c>
       <c r="AB62" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AC62" t="n">
-        <v>1419.8</v>
+        <v>0</v>
       </c>
       <c r="AD62" t="n">
         <v>1</v>
@@ -6400,58 +6400,58 @@
         <v>420</v>
       </c>
       <c r="H63" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I63" t="n">
+        <v>156.24</v>
+      </c>
+      <c r="J63" t="n">
+        <v>1</v>
+      </c>
+      <c r="K63" t="n">
         <v>64.58</v>
       </c>
-      <c r="J63" t="n">
-        <v>0</v>
-      </c>
-      <c r="K63" t="n">
-        <v>0</v>
-      </c>
       <c r="L63" t="n">
+        <v>0</v>
+      </c>
+      <c r="M63" t="n">
+        <v>0</v>
+      </c>
+      <c r="N63" t="n">
         <v>2</v>
       </c>
-      <c r="M63" t="n">
+      <c r="O63" t="n">
         <v>135.84</v>
       </c>
-      <c r="N63" t="n">
-        <v>0</v>
-      </c>
-      <c r="O63" t="n">
-        <v>0</v>
-      </c>
       <c r="P63" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q63" t="n">
-        <v>156.24</v>
+        <v>0</v>
       </c>
       <c r="R63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S63" t="n">
         <v>0</v>
       </c>
       <c r="T63" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="U63" t="n">
-        <v>0</v>
+        <v>1455.97</v>
       </c>
       <c r="V63" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="W63" t="n">
-        <v>1455.97</v>
+        <v>0</v>
       </c>
       <c r="X63" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Y63" t="n">
-        <v>0</v>
+        <v>969.78</v>
       </c>
       <c r="Z63" t="n">
         <v>0</v>
@@ -6460,13 +6460,13 @@
         <v>0</v>
       </c>
       <c r="AB63" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AC63" t="n">
-        <v>969.78</v>
+        <v>0</v>
       </c>
       <c r="AD63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE63" t="n">
         <v>0</v>

</xml_diff>